<commit_message>
Sample player stats - Luka 2022-23, updated scraping code
</commit_message>
<xml_diff>
--- a/Luka_Doncic_1629029_2022_23_game_logs.xlsx
+++ b/Luka_Doncic_1629029_2022_23_game_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Northwestern\2023-01 Winter\MSDS-456-DL\Final Project\MSDS-546-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{261F81F8-041F-4F74-A0DA-E1D29CFE57E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D25A6C1B-48EC-4A82-B4C2-664000AA76FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="1590" windowWidth="34710" windowHeight="17490"/>
+    <workbookView xWindow="21045" yWindow="2460" windowWidth="29190" windowHeight="17490"/>
   </bookViews>
   <sheets>
     <sheet name="Luka_Doncic_1629029_2022_23_gam" sheetId="1" r:id="rId1"/>
@@ -1321,20 +1321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="38" max="38" width="15.7109375" customWidth="1"/>
-    <col min="39" max="39" width="13.28515625" customWidth="1"/>
-    <col min="49" max="49" width="12.85546875" customWidth="1"/>
-    <col min="50" max="50" width="19.7109375" customWidth="1"/>
-    <col min="51" max="51" width="16.5703125" customWidth="1"/>
-    <col min="52" max="52" width="17.5703125" customWidth="1"/>
-    <col min="53" max="53" width="14.7109375" customWidth="1"/>
-    <col min="54" max="54" width="18.85546875" customWidth="1"/>
-    <col min="55" max="55" width="18" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -1807,6 +1796,9 @@
         <v>0</v>
       </c>
       <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
         <v>0</v>
       </c>
       <c r="AY3">
@@ -2298,6 +2290,9 @@
       <c r="AW6">
         <v>0</v>
       </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
       <c r="AY6">
         <v>0</v>
       </c>
@@ -10001,6 +9996,9 @@
         <v>0</v>
       </c>
       <c r="AW53">
+        <v>0</v>
+      </c>
+      <c r="AX53">
         <v>0</v>
       </c>
       <c r="AY53">

</xml_diff>